<commit_message>
Added New for real
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -33,19 +33,19 @@
     <t xml:space="preserve">what are the things you were intreseted in your childhood but due to xyz reason you have it leave it?</t>
   </si>
   <si>
-    <t xml:space="preserve">if you can make 1 rule that everyone has to follow then what would it be and why?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">are you sure that canabilism wont come in practise?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">whats the moment of your life u forget?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">whats a memory u have which you wanted to share but couldn't?</t>
-  </si>
-  <si>
     <t xml:space="preserve">what a belief that divides the world by 50 - 50?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What's the best Instgram comment you read, Explain?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What's your "It always happen to good people" moment?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is guilt over ex good or bad?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What's your secret Eureka Moment?</t>
   </si>
 </sst>
 </file>
@@ -68,7 +68,6 @@
     <font>
       <b/>
       <sz val="12.000000"/>
-      <color indexed="64"/>
       <name val="Arial"/>
     </font>
   </fonts>

</xml_diff>